<commit_message>
Update LSA Data Dictionary FY2022.xlsx
Closes #952
</commit_message>
<xml_diff>
--- a/LSA Data Dictionary FY2022.xlsx
+++ b/LSA Data Dictionary FY2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://squarepegdata-my.sharepoint.com/personal/molly_squarepegdata_com/Documents/LSA2022/Minimal Changes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://squarepegdata-my.sharepoint.com/personal/molly_squarepegdata_com/Documents/GitHub/LSASampleCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{C0152BC4-A70F-4ABE-8900-222A861E7D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A6F24A7-AE20-431B-8793-985494E95E06}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{C0152BC4-A70F-4ABE-8900-222A861E7D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319DC54D-8342-4D72-856D-843DAD47A1FF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3735" windowWidth="29040" windowHeight="15840" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
+    <workbookView xWindow="-28800" yWindow="-2100" windowWidth="20895" windowHeight="13230" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -30566,7 +30566,7 @@
         <v>655</v>
       </c>
       <c r="C85" s="14">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D85" s="14">
         <v>10</v>
@@ -30592,7 +30592,7 @@
         <v>656</v>
       </c>
       <c r="C86" s="14">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D86" s="14">
         <v>10</v>
@@ -30618,7 +30618,7 @@
         <v>657</v>
       </c>
       <c r="C87" s="14">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D87" s="14">
         <v>10</v>
@@ -30644,7 +30644,7 @@
         <v>658</v>
       </c>
       <c r="C88" s="14">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D88" s="14">
         <v>10</v>

</xml_diff>